<commit_message>
Adding Databricks_Notes Excel file & Modified SQL, PySpark_V2 Notes
</commit_message>
<xml_diff>
--- a/Databricks_SQL.xlsx
+++ b/Databricks_SQL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Confidential\myNotes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Confidential\data-cloudops-natvie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87B8AA8-16C9-47D9-B487-84FBD317E17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9339D0A9-AC55-4CF9-BF24-5330CB36F315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="2" xr2:uid="{CF404CF1-3C4E-4BE4-AB9E-1401FD2296E7}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="1" xr2:uid="{CF404CF1-3C4E-4BE4-AB9E-1401FD2296E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Date-Time Functions" sheetId="1" r:id="rId1"/>
@@ -10036,26 +10036,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -10067,6 +10055,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -10093,6 +10084,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -10105,8 +10099,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10469,7 +10469,7 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -10492,7 +10492,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="6" t="s">
         <v>42</v>
       </c>
@@ -10513,7 +10513,7 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="22" t="s">
         <v>80</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -10536,7 +10536,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="20"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="7" t="s">
         <v>54</v>
       </c>
@@ -10557,7 +10557,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="20"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="7" t="s">
         <v>59</v>
       </c>
@@ -10578,7 +10578,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="20"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="7" t="s">
         <v>64</v>
       </c>
@@ -10599,7 +10599,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="20"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="7" t="s">
         <v>69</v>
       </c>
@@ -10620,7 +10620,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="20"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="7" t="s">
         <v>74</v>
       </c>
@@ -10650,7 +10650,7 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="22" t="s">
         <v>97</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -10673,7 +10673,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="20"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="7" t="s">
         <v>87</v>
       </c>
@@ -10694,7 +10694,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="20"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="7" t="s">
         <v>92</v>
       </c>
@@ -10715,7 +10715,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="22" t="s">
         <v>98</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -10738,7 +10738,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="20"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="7" t="s">
         <v>12</v>
       </c>
@@ -10759,7 +10759,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="20"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="7" t="s">
         <v>17</v>
       </c>
@@ -10780,7 +10780,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="20"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="7" t="s">
         <v>21</v>
       </c>
@@ -10801,7 +10801,7 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="20"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="7" t="s">
         <v>26</v>
       </c>
@@ -10822,7 +10822,7 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="20"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="7" t="s">
         <v>30</v>
       </c>
@@ -10843,7 +10843,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="22" t="s">
         <v>109</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -10866,7 +10866,7 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="20"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="7" t="s">
         <v>104</v>
       </c>
@@ -10887,7 +10887,7 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="22" t="s">
         <v>135</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -10910,7 +10910,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="20"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="7" t="s">
         <v>115</v>
       </c>
@@ -10931,7 +10931,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="20"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="7" t="s">
         <v>120</v>
       </c>
@@ -10952,7 +10952,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="20"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="7" t="s">
         <v>124</v>
       </c>
@@ -10973,7 +10973,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="20"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="7" t="s">
         <v>129</v>
       </c>
@@ -10994,7 +10994,7 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="22" t="s">
         <v>149</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -11017,7 +11017,7 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="20"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="7" t="s">
         <v>140</v>
       </c>
@@ -11038,7 +11038,7 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="20"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="7" t="s">
         <v>145</v>
       </c>
@@ -11079,16 +11079,16 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="39.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.53125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.9296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.46484375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="51.86328125" bestFit="1" customWidth="1"/>
@@ -11120,7 +11120,7 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>164</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -11143,7 +11143,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="7" t="s">
         <v>156</v>
       </c>
@@ -11164,7 +11164,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="20"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="7" t="s">
         <v>160</v>
       </c>
@@ -11185,13 +11185,13 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="22" t="s">
         <v>274</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="21" t="s">
         <v>166</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -11208,11 +11208,11 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="20"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="21" t="s">
         <v>172</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -11229,11 +11229,11 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="20"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="21" t="s">
         <v>177</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -11250,11 +11250,11 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="20"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="21" t="s">
         <v>183</v>
       </c>
       <c r="D9" s="8" t="s">
@@ -11271,7 +11271,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="20"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="7" t="s">
         <v>186</v>
       </c>
@@ -11292,7 +11292,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="20"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="7" t="s">
         <v>190</v>
       </c>
@@ -11313,7 +11313,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="20"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="7" t="s">
         <v>195</v>
       </c>
@@ -11334,13 +11334,13 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="22" t="s">
         <v>273</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="21" t="s">
         <v>200</v>
       </c>
       <c r="D14" s="8" t="s">
@@ -11357,11 +11357,11 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="20"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="21" t="s">
         <v>203</v>
       </c>
       <c r="D15" s="8" t="s">
@@ -11378,8 +11378,8 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="20"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="22"/>
+      <c r="B16" s="21" t="s">
         <v>207</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -11399,7 +11399,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="22" t="s">
         <v>272</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -11422,7 +11422,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="20"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="7" t="s">
         <v>216</v>
       </c>
@@ -11443,7 +11443,7 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="20"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="7" t="s">
         <v>220</v>
       </c>
@@ -11464,7 +11464,7 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="20"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="7" t="s">
         <v>224</v>
       </c>
@@ -11485,7 +11485,7 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="20"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="7" t="s">
         <v>228</v>
       </c>
@@ -11506,7 +11506,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="20"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="7" t="s">
         <v>234</v>
       </c>
@@ -11527,7 +11527,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="22" t="s">
         <v>271</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -11550,7 +11550,7 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="20"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="7" t="s">
         <v>243</v>
       </c>
@@ -11571,7 +11571,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="20"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="7" t="s">
         <v>247</v>
       </c>
@@ -11592,7 +11592,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="20"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="7" t="s">
         <v>251</v>
       </c>
@@ -11613,7 +11613,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="20"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="7" t="s">
         <v>256</v>
       </c>
@@ -11634,7 +11634,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="20"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="7" t="s">
         <v>261</v>
       </c>
@@ -11696,7 +11696,7 @@
   </sheetPr>
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
@@ -11747,7 +11747,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>1302</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -11779,7 +11779,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="15" t="s">
         <v>1297</v>
       </c>
@@ -11809,7 +11809,7 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="20"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="15" t="s">
         <v>1292</v>
       </c>
@@ -11839,7 +11839,7 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="20"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="15" t="s">
         <v>1287</v>
       </c>
@@ -11869,7 +11869,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="20"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="15" t="s">
         <v>1283</v>
       </c>
@@ -11899,7 +11899,7 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="22" t="s">
         <v>1278</v>
       </c>
       <c r="B8" s="15" t="s">
@@ -11931,7 +11931,7 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="20"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="15" t="s">
         <v>1273</v>
       </c>
@@ -11961,7 +11961,7 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="20"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="15" t="s">
         <v>1269</v>
       </c>
@@ -11991,7 +11991,7 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="20"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="15" t="s">
         <v>1265</v>
       </c>
@@ -12021,7 +12021,7 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="22" t="s">
         <v>1259</v>
       </c>
       <c r="B13" s="15" t="s">
@@ -12053,7 +12053,7 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="20"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="15" t="s">
         <v>1254</v>
       </c>
@@ -12083,7 +12083,7 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="41" t="s">
         <v>1249</v>
       </c>
       <c r="B16" s="15" t="s">
@@ -12115,7 +12115,7 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="15" t="s">
         <v>1244</v>
       </c>
@@ -12145,7 +12145,7 @@
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="23"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="15" t="s">
         <v>1238</v>
       </c>
@@ -12208,285 +12208,285 @@
     </row>
     <row r="22" spans="1:10" ht="14.65" thickBot="1"/>
     <row r="23" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="32" t="s">
         <v>1311</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="38"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="38"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="38"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
     </row>
     <row r="27" spans="1:10" ht="14.65" thickBot="1">
-      <c r="A27" s="40"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10" ht="14.65" thickBot="1"/>
     <row r="29" spans="1:10">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="23" t="s">
         <v>1312</v>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="29"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="25"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="30"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="31"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="28"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="30"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="31"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="28"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="30"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="31"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="28"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="30"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="31"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="28"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="30"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="31"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="28"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="30"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="31"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="28"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="30"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="31"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="28"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="30"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="31"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="28"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="30"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="31"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="28"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="30"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="31"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="28"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="30"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="31"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="28"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="30"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="31"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="28"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="30"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="31"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="28"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="30"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="31"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="28"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="30"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="31"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="28"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="30"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="31"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="28"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="30"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="31"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="28"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="30"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="31"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="28"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="30"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="31"/>
+      <c r="A48" s="26"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="28"/>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="30"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="31"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="28"/>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="30"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="31"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="28"/>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="30"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="31"/>
+      <c r="A51" s="26"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="28"/>
     </row>
     <row r="52" spans="1:7" ht="14.65" thickBot="1">
-      <c r="A52" s="32"/>
-      <c r="B52" s="33"/>
-      <c r="C52" s="33"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="34"/>
+      <c r="A52" s="29"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -12548,7 +12548,7 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>294</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -12571,7 +12571,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="13" t="s">
         <v>279</v>
       </c>
@@ -12592,7 +12592,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="20"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="13" t="s">
         <v>284</v>
       </c>
@@ -12613,7 +12613,7 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="20"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="13" t="s">
         <v>289</v>
       </c>
@@ -12634,7 +12634,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="22" t="s">
         <v>337</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -12657,7 +12657,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="20"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="7" t="s">
         <v>300</v>
       </c>
@@ -12678,7 +12678,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="20"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="7" t="s">
         <v>304</v>
       </c>
@@ -12699,7 +12699,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="20"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="7" t="s">
         <v>309</v>
       </c>
@@ -12720,7 +12720,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="20"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="7" t="s">
         <v>314</v>
       </c>
@@ -12741,7 +12741,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="20"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="7" t="s">
         <v>319</v>
       </c>
@@ -12762,7 +12762,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="20"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="7" t="s">
         <v>324</v>
       </c>
@@ -12783,7 +12783,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="20"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="7" t="s">
         <v>328</v>
       </c>
@@ -12804,7 +12804,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="20"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="7" t="s">
         <v>332</v>
       </c>
@@ -12825,7 +12825,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="22" t="s">
         <v>349</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -12848,7 +12848,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="20"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="7" t="s">
         <v>344</v>
       </c>
@@ -12869,7 +12869,7 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="22" t="s">
         <v>361</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -12892,7 +12892,7 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="20"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="7" t="s">
         <v>354</v>
       </c>
@@ -12913,7 +12913,7 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="20"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="7" t="s">
         <v>358</v>
       </c>
@@ -12934,7 +12934,7 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="22" t="s">
         <v>384</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -12957,7 +12957,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="20"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="7" t="s">
         <v>367</v>
       </c>
@@ -12978,7 +12978,7 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="20"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="7" t="s">
         <v>371</v>
       </c>
@@ -12999,7 +12999,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="20"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="7" t="s">
         <v>376</v>
       </c>
@@ -13020,7 +13020,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="20"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="7" t="s">
         <v>380</v>
       </c>
@@ -13041,7 +13041,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="22" t="s">
         <v>406</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -13064,7 +13064,7 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="20"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="7" t="s">
         <v>389</v>
       </c>
@@ -13085,7 +13085,7 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="20"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="7" t="s">
         <v>394</v>
       </c>
@@ -13106,7 +13106,7 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="20"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="7" t="s">
         <v>398</v>
       </c>
@@ -13127,7 +13127,7 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="20"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="7" t="s">
         <v>402</v>
       </c>
@@ -13217,7 +13217,7 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="20" t="s">
+      <c r="A42" s="22" t="s">
         <v>442</v>
       </c>
       <c r="B42" s="7" t="s">
@@ -13240,7 +13240,7 @@
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="20"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="7" t="s">
         <v>429</v>
       </c>
@@ -13261,7 +13261,7 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="20"/>
+      <c r="A44" s="22"/>
       <c r="B44" s="7" t="s">
         <v>433</v>
       </c>
@@ -13282,7 +13282,7 @@
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="20"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="7" t="s">
         <v>437</v>
       </c>
@@ -13303,7 +13303,7 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="20" t="s">
+      <c r="A47" s="22" t="s">
         <v>461</v>
       </c>
       <c r="B47" s="7" t="s">
@@ -13326,7 +13326,7 @@
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="20"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="7" t="s">
         <v>448</v>
       </c>
@@ -13347,7 +13347,7 @@
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="20"/>
+      <c r="A49" s="22"/>
       <c r="B49" s="7" t="s">
         <v>452</v>
       </c>
@@ -13368,7 +13368,7 @@
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="20"/>
+      <c r="A50" s="22"/>
       <c r="B50" s="7" t="s">
         <v>457</v>
       </c>
@@ -13389,7 +13389,7 @@
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="20" t="s">
+      <c r="A52" s="22" t="s">
         <v>470</v>
       </c>
       <c r="B52" s="7" t="s">
@@ -13412,7 +13412,7 @@
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="20"/>
+      <c r="A53" s="22"/>
       <c r="B53" s="7" t="s">
         <v>466</v>
       </c>
@@ -13433,7 +13433,7 @@
       </c>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="20" t="s">
+      <c r="A55" s="22" t="s">
         <v>480</v>
       </c>
       <c r="B55" s="7" t="s">
@@ -13456,7 +13456,7 @@
       </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="20"/>
+      <c r="A56" s="22"/>
       <c r="B56" s="7" t="s">
         <v>476</v>
       </c>
@@ -13540,7 +13540,7 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>502</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -13563,7 +13563,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="7" t="s">
         <v>487</v>
       </c>
@@ -13584,7 +13584,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="20"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="7" t="s">
         <v>492</v>
       </c>
@@ -13605,7 +13605,7 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="20"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="7" t="s">
         <v>497</v>
       </c>
@@ -13626,7 +13626,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="22" t="s">
         <v>509</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -13649,7 +13649,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="20"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="7" t="s">
         <v>358</v>
       </c>
@@ -13670,7 +13670,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="22" t="s">
         <v>521</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -13693,7 +13693,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="20"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="7" t="s">
         <v>371</v>
       </c>
@@ -13714,7 +13714,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="20"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="7" t="s">
         <v>380</v>
       </c>
@@ -13735,7 +13735,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="22" t="s">
         <v>530</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -13758,7 +13758,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="20"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="7" t="s">
         <v>526</v>
       </c>
@@ -13779,7 +13779,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="22" t="s">
         <v>549</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -13802,7 +13802,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="20"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="7" t="s">
         <v>536</v>
       </c>
@@ -13823,7 +13823,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="20"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="7" t="s">
         <v>540</v>
       </c>
@@ -13844,7 +13844,7 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="20"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="7" t="s">
         <v>544</v>
       </c>
@@ -13888,7 +13888,7 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="22" t="s">
         <v>562</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -13911,7 +13911,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="20"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="7" t="s">
         <v>448</v>
       </c>
@@ -14014,7 +14014,7 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>648</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -14037,7 +14037,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="25.5">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="6" t="s">
         <v>574</v>
       </c>
@@ -14058,7 +14058,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="20"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="6" t="s">
         <v>579</v>
       </c>
@@ -14079,7 +14079,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="22" t="s">
         <v>649</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -14102,7 +14102,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="20"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="7" t="s">
         <v>592</v>
       </c>
@@ -14123,7 +14123,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="20"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="7" t="s">
         <v>597</v>
       </c>
@@ -14144,7 +14144,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="20"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="7" t="s">
         <v>602</v>
       </c>
@@ -14165,7 +14165,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="20"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="7" t="s">
         <v>606</v>
       </c>
@@ -14186,7 +14186,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="20"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="7" t="s">
         <v>612</v>
       </c>
@@ -14207,7 +14207,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="20"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="7" t="s">
         <v>618</v>
       </c>
@@ -14228,7 +14228,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="22" t="s">
         <v>650</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -14251,7 +14251,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="20"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="7" t="s">
         <v>627</v>
       </c>
@@ -14272,7 +14272,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="20"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="7" t="s">
         <v>631</v>
       </c>
@@ -14293,7 +14293,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="20"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="7" t="s">
         <v>635</v>
       </c>
@@ -14314,7 +14314,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="20"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="7" t="s">
         <v>639</v>
       </c>
@@ -14335,7 +14335,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="20"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="7" t="s">
         <v>644</v>
       </c>
@@ -14356,7 +14356,7 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="22" t="s">
         <v>746</v>
       </c>
       <c r="B21" s="9" t="s">
@@ -14379,7 +14379,7 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="20"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="9" t="s">
         <v>655</v>
       </c>
@@ -14400,7 +14400,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="20"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="9" t="s">
         <v>659</v>
       </c>
@@ -14421,7 +14421,7 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="20"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="9" t="s">
         <v>663</v>
       </c>
@@ -14442,7 +14442,7 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="22" t="s">
         <v>745</v>
       </c>
       <c r="B26" s="9" t="s">
@@ -14465,7 +14465,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="20"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="9" t="s">
         <v>672</v>
       </c>
@@ -14486,7 +14486,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="22" t="s">
         <v>744</v>
       </c>
       <c r="B29" s="9" t="s">
@@ -14509,7 +14509,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="20"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="9" t="s">
         <v>682</v>
       </c>
@@ -14553,7 +14553,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="25.5">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="22" t="s">
         <v>742</v>
       </c>
       <c r="B34" s="11" t="s">
@@ -14576,7 +14576,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="25.5">
-      <c r="A35" s="20"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="11" t="s">
         <v>698</v>
       </c>
@@ -14597,7 +14597,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="25.5">
-      <c r="A36" s="20"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="11" t="s">
         <v>703</v>
       </c>
@@ -14618,7 +14618,7 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="20"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="11" t="s">
         <v>707</v>
       </c>
@@ -14639,7 +14639,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="28.5">
-      <c r="A38" s="20"/>
+      <c r="A38" s="22"/>
       <c r="B38" s="11" t="s">
         <v>712</v>
       </c>
@@ -14683,7 +14683,7 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="20" t="s">
+      <c r="A42" s="22" t="s">
         <v>740</v>
       </c>
       <c r="B42" s="9" t="s">
@@ -14706,7 +14706,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="28.5">
-      <c r="A43" s="20"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="9" t="s">
         <v>727</v>
       </c>
@@ -14811,7 +14811,7 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>850</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -14834,7 +14834,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="7" t="s">
         <v>752</v>
       </c>
@@ -14855,7 +14855,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="20"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="7" t="s">
         <v>757</v>
       </c>
@@ -14876,7 +14876,7 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="20"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="7" t="s">
         <v>762</v>
       </c>
@@ -14897,7 +14897,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="20"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="7" t="s">
         <v>767</v>
       </c>
@@ -14918,7 +14918,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="20"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="7" t="s">
         <v>772</v>
       </c>
@@ -14939,7 +14939,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="20"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="7" t="s">
         <v>777</v>
       </c>
@@ -14960,7 +14960,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="20"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="7" t="s">
         <v>782</v>
       </c>
@@ -14981,7 +14981,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="20"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="7" t="s">
         <v>787</v>
       </c>
@@ -15002,7 +15002,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="20"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="7" t="s">
         <v>792</v>
       </c>
@@ -15023,7 +15023,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="20"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="7" t="s">
         <v>797</v>
       </c>
@@ -15044,7 +15044,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="22" t="s">
         <v>849</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -15067,7 +15067,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="20"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="7" t="s">
         <v>807</v>
       </c>
@@ -15088,7 +15088,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="20"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="7" t="s">
         <v>812</v>
       </c>
@@ -15109,7 +15109,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="20"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="7" t="s">
         <v>818</v>
       </c>
@@ -15130,7 +15130,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="20"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="7" t="s">
         <v>822</v>
       </c>
@@ -15151,7 +15151,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="20"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="7" t="s">
         <v>826</v>
       </c>
@@ -15172,7 +15172,7 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="20"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="7" t="s">
         <v>830</v>
       </c>
@@ -15193,7 +15193,7 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="20"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="7" t="s">
         <v>835</v>
       </c>
@@ -15214,7 +15214,7 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="20"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="7" t="s">
         <v>839</v>
       </c>
@@ -15235,7 +15235,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="20"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="7" t="s">
         <v>844</v>
       </c>
@@ -15256,7 +15256,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="22" t="s">
         <v>882</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -15279,7 +15279,7 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="20"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="7" t="s">
         <v>856</v>
       </c>
@@ -15300,7 +15300,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="20"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="7" t="s">
         <v>860</v>
       </c>
@@ -15321,7 +15321,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="20"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="7" t="s">
         <v>865</v>
       </c>
@@ -15342,7 +15342,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="20"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="7" t="s">
         <v>870</v>
       </c>
@@ -15363,7 +15363,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="20"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="7" t="s">
         <v>874</v>
       </c>
@@ -15384,7 +15384,7 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="20"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="7" t="s">
         <v>877</v>
       </c>
@@ -15405,7 +15405,7 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="22" t="s">
         <v>917</v>
       </c>
       <c r="B33" s="7" t="s">
@@ -15428,7 +15428,7 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="20"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="7" t="s">
         <v>887</v>
       </c>
@@ -15449,7 +15449,7 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="20"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="7" t="s">
         <v>891</v>
       </c>
@@ -15470,7 +15470,7 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="20"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="7" t="s">
         <v>895</v>
       </c>
@@ -15491,7 +15491,7 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="20"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="7" t="s">
         <v>899</v>
       </c>
@@ -15512,7 +15512,7 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="20"/>
+      <c r="A38" s="22"/>
       <c r="B38" s="7" t="s">
         <v>324</v>
       </c>
@@ -15533,7 +15533,7 @@
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="20"/>
+      <c r="A39" s="22"/>
       <c r="B39" s="7" t="s">
         <v>906</v>
       </c>
@@ -15554,7 +15554,7 @@
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="20"/>
+      <c r="A40" s="22"/>
       <c r="B40" s="7" t="s">
         <v>911</v>
       </c>
@@ -15575,7 +15575,7 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="20"/>
+      <c r="A41" s="22"/>
       <c r="B41" s="7" t="s">
         <v>916</v>
       </c>
@@ -15596,7 +15596,7 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="20"/>
+      <c r="A42" s="22"/>
       <c r="B42" s="7" t="s">
         <v>922</v>
       </c>
@@ -15617,7 +15617,7 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="22" t="s">
         <v>1000</v>
       </c>
       <c r="B44" s="7" t="s">
@@ -15640,7 +15640,7 @@
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="20"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="7" t="s">
         <v>932</v>
       </c>
@@ -15661,7 +15661,7 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="20"/>
+      <c r="A46" s="22"/>
       <c r="B46" s="7" t="s">
         <v>937</v>
       </c>
@@ -15682,7 +15682,7 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="20"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="7" t="s">
         <v>942</v>
       </c>
@@ -15703,7 +15703,7 @@
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="20"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="7" t="s">
         <v>947</v>
       </c>
@@ -15724,7 +15724,7 @@
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="20"/>
+      <c r="A49" s="22"/>
       <c r="B49" s="7" t="s">
         <v>951</v>
       </c>
@@ -15745,7 +15745,7 @@
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="20"/>
+      <c r="A50" s="22"/>
       <c r="B50" s="7" t="s">
         <v>956</v>
       </c>
@@ -15766,7 +15766,7 @@
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="20"/>
+      <c r="A51" s="22"/>
       <c r="B51" s="7" t="s">
         <v>961</v>
       </c>
@@ -15787,7 +15787,7 @@
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="20"/>
+      <c r="A52" s="22"/>
       <c r="B52" s="7" t="s">
         <v>966</v>
       </c>
@@ -15808,7 +15808,7 @@
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="20"/>
+      <c r="A53" s="22"/>
       <c r="B53" s="7" t="s">
         <v>971</v>
       </c>
@@ -15829,7 +15829,7 @@
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="20"/>
+      <c r="A54" s="22"/>
       <c r="B54" s="7" t="s">
         <v>975</v>
       </c>
@@ -15850,7 +15850,7 @@
       </c>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="20"/>
+      <c r="A55" s="22"/>
       <c r="B55" s="7" t="s">
         <v>979</v>
       </c>
@@ -15871,7 +15871,7 @@
       </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="20"/>
+      <c r="A56" s="22"/>
       <c r="B56" s="7" t="s">
         <v>984</v>
       </c>
@@ -15892,7 +15892,7 @@
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="20"/>
+      <c r="A57" s="22"/>
       <c r="B57" s="7" t="s">
         <v>989</v>
       </c>
@@ -15913,7 +15913,7 @@
       </c>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="20"/>
+      <c r="A58" s="22"/>
       <c r="B58" s="7" t="s">
         <v>995</v>
       </c>
@@ -15934,7 +15934,7 @@
       </c>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="20" t="s">
+      <c r="A60" s="22" t="s">
         <v>1036</v>
       </c>
       <c r="B60" s="7" t="s">
@@ -15957,7 +15957,7 @@
       </c>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="20"/>
+      <c r="A61" s="22"/>
       <c r="B61" s="7" t="s">
         <v>733</v>
       </c>
@@ -15978,7 +15978,7 @@
       </c>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="20"/>
+      <c r="A62" s="22"/>
       <c r="B62" s="7" t="s">
         <v>1010</v>
       </c>
@@ -15999,7 +15999,7 @@
       </c>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="20"/>
+      <c r="A63" s="22"/>
       <c r="B63" s="7" t="s">
         <v>1015</v>
       </c>
@@ -16020,7 +16020,7 @@
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="20"/>
+      <c r="A64" s="22"/>
       <c r="B64" s="7" t="s">
         <v>1019</v>
       </c>
@@ -16041,7 +16041,7 @@
       </c>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="20"/>
+      <c r="A65" s="22"/>
       <c r="B65" s="7" t="s">
         <v>1023</v>
       </c>
@@ -16062,7 +16062,7 @@
       </c>
     </row>
     <row r="66" spans="1:7">
-      <c r="A66" s="20"/>
+      <c r="A66" s="22"/>
       <c r="B66" s="7" t="s">
         <v>1028</v>
       </c>
@@ -16083,7 +16083,7 @@
       </c>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="20"/>
+      <c r="A67" s="22"/>
       <c r="B67" s="7" t="s">
         <v>792</v>
       </c>
@@ -16104,7 +16104,7 @@
       </c>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="20" t="s">
+      <c r="A69" s="22" t="s">
         <v>1067</v>
       </c>
       <c r="B69" s="9" t="s">
@@ -16127,7 +16127,7 @@
       </c>
     </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="20"/>
+      <c r="A70" s="22"/>
       <c r="B70" s="9" t="s">
         <v>1041</v>
       </c>
@@ -16148,7 +16148,7 @@
       </c>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="20"/>
+      <c r="A71" s="22"/>
       <c r="B71" s="9" t="s">
         <v>1045</v>
       </c>
@@ -16169,7 +16169,7 @@
       </c>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="20"/>
+      <c r="A72" s="22"/>
       <c r="B72" s="9" t="s">
         <v>1049</v>
       </c>
@@ -16190,7 +16190,7 @@
       </c>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="20"/>
+      <c r="A73" s="22"/>
       <c r="B73" s="9" t="s">
         <v>1054</v>
       </c>
@@ -16211,7 +16211,7 @@
       </c>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="20"/>
+      <c r="A74" s="22"/>
       <c r="B74" s="9" t="s">
         <v>667</v>
       </c>
@@ -16232,7 +16232,7 @@
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="20"/>
+      <c r="A75" s="22"/>
       <c r="B75" s="9" t="s">
         <v>1063</v>
       </c>
@@ -16253,7 +16253,7 @@
       </c>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="20" t="s">
+      <c r="A77" s="22" t="s">
         <v>1083</v>
       </c>
       <c r="B77" s="9" t="s">
@@ -16276,7 +16276,7 @@
       </c>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="20"/>
+      <c r="A78" s="22"/>
       <c r="B78" s="9" t="s">
         <v>1073</v>
       </c>
@@ -16297,7 +16297,7 @@
       </c>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="20"/>
+      <c r="A79" s="22"/>
       <c r="B79" s="9" t="s">
         <v>1078</v>
       </c>
@@ -16341,7 +16341,7 @@
       </c>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="20" t="s">
+      <c r="A83" s="22" t="s">
         <v>1098</v>
       </c>
       <c r="B83" s="7" t="s">
@@ -16364,7 +16364,7 @@
       </c>
     </row>
     <row r="84" spans="1:7">
-      <c r="A84" s="20"/>
+      <c r="A84" s="22"/>
       <c r="B84" s="7" t="s">
         <v>1092</v>
       </c>
@@ -16385,7 +16385,7 @@
       </c>
     </row>
     <row r="85" spans="1:7">
-      <c r="A85" s="20"/>
+      <c r="A85" s="22"/>
       <c r="B85" s="7" t="s">
         <v>1054</v>
       </c>
@@ -16468,7 +16468,7 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>1126</v>
       </c>
       <c r="B2" s="16" t="s">
@@ -16491,7 +16491,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="16" t="s">
         <v>1105</v>
       </c>
@@ -16512,7 +16512,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="20"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="16" t="s">
         <v>1110</v>
       </c>
@@ -16533,7 +16533,7 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="20"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="16" t="s">
         <v>1115</v>
       </c>
@@ -16554,7 +16554,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="20"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="16" t="s">
         <v>1120</v>
       </c>

</xml_diff>